<commit_message>
Refractored excel generation. Started working on configuration in form size.
Split the excel generation from the xml generation to have reusability on xml side.
</commit_message>
<xml_diff>
--- a/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAppoggi.xlsx
+++ b/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAppoggi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PARONETTO G\Documents\GitHub\TiaAddIn-Spin\TiaAddin-Spin-ExcelReader\z.Excel Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5C908C-B492-44FB-B380-505DB0AC001F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9A1224-1CAA-4875-BBEE-ABBEFA09D5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27750" windowHeight="16440" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="20640" windowHeight="11835" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -6137,7 +6137,7 @@
   <dimension ref="A1:IH900"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:I3"/>
+      <selection activeCell="B15" sqref="B15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>